<commit_message>
cleaned up the excel file
</commit_message>
<xml_diff>
--- a/ETC3430/Assignments/Data.xlsx
+++ b/ETC3430/Assignments/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/JAY/Dropbox/My Mac (PengjieeMacBook)/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chela\GitHub Local Repo\Uni-Work\ETC3430\Assignments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A803877-AF28-934A-8BC8-C0CA55ABF8DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AF5F46D-65E9-43F4-87AE-C08EF22A075C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15740" activeTab="1" xr2:uid="{2C8865CE-5F3F-614B-A1D5-9973406A6BA4}"/>
+    <workbookView xWindow="10425" yWindow="3285" windowWidth="10605" windowHeight="11835" activeTab="1" xr2:uid="{2C8865CE-5F3F-614B-A1D5-9973406A6BA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>Dataset 1</t>
   </si>
@@ -40,12 +40,6 @@
   </si>
   <si>
     <t>X_t</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
-    <t>W_n</t>
   </si>
 </sst>
 </file>
@@ -56,13 +50,13 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -92,7 +86,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -108,7 +102,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -410,7 +404,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="2:4">
       <c r="B1" t="s">
@@ -1236,1031 +1230,747 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78A97EBA-CCCC-B648-A97B-139321C324F2}">
-  <dimension ref="A1:D93"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>2.2999147905061501</v>
+      </c>
+      <c r="B2">
+        <v>5.6200663099214596</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3">
-        <v>1</v>
+        <v>7.1753281194462604</v>
       </c>
       <c r="B3">
-        <v>2.2999147905061501</v>
-      </c>
-      <c r="D3">
-        <v>5.6200663099214596</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>3.1019719117395699</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4">
-        <v>2</v>
+        <v>32.2405957347843</v>
       </c>
       <c r="B4">
-        <v>7.1753281194462604</v>
-      </c>
-      <c r="D4">
-        <v>3.1019719117395699</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>7.9827039872027399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5">
-        <v>3</v>
+        <v>0.26900680254175102</v>
       </c>
       <c r="B5">
-        <v>32.2405957347843</v>
-      </c>
-      <c r="D5">
-        <v>7.9827039872027399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>2.7889030736154101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6">
-        <v>4</v>
+        <v>23.620131819469901</v>
       </c>
       <c r="B6">
-        <v>0.26900680254175102</v>
-      </c>
-      <c r="D6">
-        <v>2.7889030736154101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>7.76234627397802E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7">
-        <v>5</v>
+        <v>0.42274130207407801</v>
       </c>
       <c r="B7">
-        <v>23.620131819469901</v>
-      </c>
-      <c r="D7">
-        <v>7.76234627397802E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0.383959013633279</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8">
-        <v>6</v>
+        <v>59.3402561635749</v>
       </c>
       <c r="B8">
-        <v>0.42274130207407801</v>
-      </c>
-      <c r="D8">
-        <v>0.383959013633279</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>6.3247034497888102</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9">
-        <v>7</v>
+        <v>0.111242935469667</v>
       </c>
       <c r="B9">
-        <v>59.3402561635749</v>
-      </c>
-      <c r="D9">
-        <v>6.3247034497888102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.37369099719965099</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10">
-        <v>8</v>
+        <v>16.1944411331731</v>
       </c>
       <c r="B10">
-        <v>0.111242935469667</v>
-      </c>
-      <c r="D10">
-        <v>0.37369099719965099</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>4.6497859618614896</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11">
-        <v>9</v>
+        <v>0.79277719052004503</v>
       </c>
       <c r="B11">
-        <v>16.1944411331731</v>
-      </c>
-      <c r="D11">
-        <v>4.6497859618614896</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>1.5458355652118201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12">
-        <v>10</v>
+        <v>94.002321696570903</v>
       </c>
       <c r="B12">
-        <v>0.79277719052004503</v>
-      </c>
-      <c r="D12">
-        <v>1.5458355652118201</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>0.22216409034307799</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13">
-        <v>11</v>
+        <v>1.27737241206343</v>
       </c>
       <c r="B13">
-        <v>94.002321696570903</v>
-      </c>
-      <c r="D13">
-        <v>0.22216409034307799</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>0.37048184712351501</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14">
-        <v>12</v>
+        <v>19.001923094050099</v>
       </c>
       <c r="B14">
-        <v>1.27737241206343</v>
-      </c>
-      <c r="D14">
-        <v>0.37048184712351501</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>3.9167776631100599</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15">
-        <v>13</v>
+        <v>1.0589926624069601</v>
       </c>
       <c r="B15">
-        <v>19.001923094050099</v>
-      </c>
-      <c r="D15">
-        <v>3.9167776631100599</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>3.2031850789579499</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16">
-        <v>14</v>
+        <v>40.221691381486103</v>
       </c>
       <c r="B16">
-        <v>1.0589926624069601</v>
-      </c>
-      <c r="D16">
-        <v>3.2031850789579499</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>3.5443094378161599</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17">
-        <v>15</v>
+        <v>0.62444063221440904</v>
       </c>
       <c r="B17">
-        <v>40.221691381486103</v>
-      </c>
-      <c r="D17">
-        <v>3.5443094378161599</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>9.5128089494646897</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18">
-        <v>16</v>
+        <v>32.151677892776704</v>
       </c>
       <c r="B18">
-        <v>0.62444063221440904</v>
-      </c>
-      <c r="D18">
-        <v>9.5128089494646897</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>4.94535612050902</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19">
-        <v>17</v>
+        <v>0.55770846707762001</v>
       </c>
       <c r="B19">
-        <v>32.151677892776704</v>
-      </c>
-      <c r="D19">
-        <v>4.94535612050902</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>0.42064425586783499</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20">
-        <v>18</v>
+        <v>24.532419745887601</v>
       </c>
       <c r="B20">
-        <v>0.55770846707762001</v>
-      </c>
-      <c r="D20">
-        <v>0.42064425586783499</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>15.0262567281738</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21">
-        <v>19</v>
+        <v>0.28086344990083201</v>
       </c>
       <c r="B21">
-        <v>24.532419745887601</v>
-      </c>
-      <c r="D21">
-        <v>15.0262567281738</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>0.94359684623037299</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22">
-        <v>20</v>
+        <v>31.359168319914399</v>
       </c>
       <c r="B22">
-        <v>0.28086344990083201</v>
-      </c>
-      <c r="D22">
-        <v>0.94359684623037299</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>1.8123571459082199</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23">
-        <v>21</v>
+        <v>0.12419806211557501</v>
       </c>
       <c r="B23">
-        <v>31.359168319914399</v>
-      </c>
-      <c r="D23">
-        <v>1.8123571459082199</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>4.1449556603237001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24">
-        <v>22</v>
+        <v>55.022510863010403</v>
       </c>
       <c r="B24">
-        <v>0.12419806211557501</v>
-      </c>
-      <c r="D24">
-        <v>4.1449556603237001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>3.4575739386673798</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25">
-        <v>23</v>
+        <v>3.11524750373305</v>
       </c>
       <c r="B25">
-        <v>55.022510863010403</v>
-      </c>
-      <c r="D25">
-        <v>3.4575739386673798</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>6.0932445820194898</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26">
-        <v>24</v>
+        <v>57.905017973427697</v>
       </c>
       <c r="B26">
-        <v>3.11524750373305</v>
-      </c>
-      <c r="D26">
-        <v>6.0932445820194898</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>0.416969316763176</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27">
-        <v>25</v>
+        <v>2.8155528256511402</v>
       </c>
       <c r="B27">
-        <v>57.905017973427697</v>
-      </c>
-      <c r="D27">
-        <v>0.416969316763176</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>3.5449619644943399E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28">
-        <v>26</v>
+        <v>9.0555157900939296</v>
       </c>
       <c r="B28">
-        <v>2.8155528256511402</v>
-      </c>
-      <c r="D28">
-        <v>3.5449619644943399E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>10.110228308865</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29">
-        <v>27</v>
+        <v>3.96698326585877</v>
       </c>
       <c r="B29">
-        <v>9.0555157900939296</v>
-      </c>
-      <c r="D29">
-        <v>10.110228308865</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>0.213322651973716</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30">
-        <v>28</v>
+        <v>22.5495109677221</v>
       </c>
       <c r="B30">
-        <v>3.96698326585877</v>
-      </c>
-      <c r="D30">
-        <v>0.213322651973716</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>1.9760928037158301</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31">
-        <v>29</v>
+        <v>0.78078484287862904</v>
       </c>
       <c r="B31">
-        <v>22.5495109677221</v>
-      </c>
-      <c r="D31">
-        <v>1.9760928037158301</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>0.54795188731310795</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32">
-        <v>30</v>
+        <v>9.6049210123319195</v>
       </c>
       <c r="B32">
-        <v>0.78078484287862904</v>
-      </c>
-      <c r="D32">
-        <v>0.54795188731310795</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>1.6587439721306001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33">
-        <v>31</v>
+        <v>2.0934408054698901</v>
       </c>
       <c r="B33">
-        <v>9.6049210123319195</v>
-      </c>
-      <c r="D33">
-        <v>1.6587439721306001</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>0.99659751586723</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34">
-        <v>32</v>
+        <v>7.4447006983173001</v>
       </c>
       <c r="B34">
-        <v>2.0934408054698901</v>
-      </c>
-      <c r="D34">
-        <v>0.99659751586723</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>13.9753298577489</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35">
-        <v>33</v>
+        <v>1.35496361925456</v>
       </c>
       <c r="B35">
-        <v>7.4447006983173001</v>
-      </c>
-      <c r="D35">
-        <v>13.9753298577489</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>2.8717464194981401</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36">
-        <v>34</v>
+        <v>13.5651965750519</v>
       </c>
       <c r="B36">
-        <v>1.35496361925456</v>
-      </c>
-      <c r="D36">
-        <v>2.8717464194981401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>2.1825239744523302</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37">
-        <v>35</v>
+        <v>1.5784942517811</v>
       </c>
       <c r="B37">
-        <v>13.5651965750519</v>
-      </c>
-      <c r="D37">
-        <v>2.1825239744523302</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>0.48309195065055399</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38">
-        <v>36</v>
+        <v>5.9449872631055696</v>
       </c>
       <c r="B38">
-        <v>1.5784942517811</v>
-      </c>
-      <c r="D38">
-        <v>0.48309195065055399</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>4.9700770926901798</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39">
-        <v>37</v>
+        <v>1.45511088554596</v>
       </c>
       <c r="B39">
-        <v>5.9449872631055696</v>
-      </c>
-      <c r="D39">
-        <v>4.9700770926901798</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>2.3042268430955199</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40">
-        <v>38</v>
+        <v>86.821407893115804</v>
       </c>
       <c r="B40">
-        <v>1.45511088554596</v>
-      </c>
-      <c r="D40">
-        <v>2.3042268430955199</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>0.57371661563800203</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41">
-        <v>39</v>
+        <v>1.2123936339941599</v>
       </c>
       <c r="B41">
-        <v>86.821407893115804</v>
-      </c>
-      <c r="D41">
-        <v>0.57371661563800203</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>4.6578795941249203E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42">
-        <v>40</v>
+        <v>114.216630591125</v>
       </c>
       <c r="B42">
-        <v>1.2123936339941599</v>
-      </c>
-      <c r="D42">
-        <v>4.6578795941249203E-2</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>0.43946433887085301</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43">
-        <v>41</v>
+        <v>0.25554026779141698</v>
       </c>
       <c r="B43">
-        <v>114.216630591125</v>
-      </c>
-      <c r="D43">
-        <v>0.43946433887085301</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>1.88260945818706</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44">
-        <v>42</v>
+        <v>91.050202719725107</v>
       </c>
       <c r="B44">
-        <v>0.25554026779141698</v>
-      </c>
-      <c r="D44">
-        <v>1.88260945818706</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>1.8419022303855099</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45">
-        <v>43</v>
+        <v>1.2404889402141599</v>
       </c>
       <c r="B45">
-        <v>91.050202719725107</v>
-      </c>
-      <c r="D45">
-        <v>1.8419022303855099</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>1.9068899036967299</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46">
-        <v>44</v>
+        <v>2.76373904708707</v>
       </c>
       <c r="B46">
-        <v>1.2404889402141599</v>
-      </c>
-      <c r="D46">
-        <v>1.9068899036967299</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>3.8734516745576602</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47">
-        <v>45</v>
+        <v>1.6143386276034299E-2</v>
       </c>
       <c r="B47">
-        <v>2.76373904708707</v>
-      </c>
-      <c r="D47">
-        <v>3.8734516745576602</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>3.17537935753636</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48">
-        <v>46</v>
+        <v>37.808246944275901</v>
       </c>
       <c r="B48">
-        <v>1.6143386276034299E-2</v>
-      </c>
-      <c r="D48">
-        <v>3.17537935753636</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>5.1613803315773499</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49">
-        <v>47</v>
+        <v>0.247642529507378</v>
       </c>
       <c r="B49">
-        <v>37.808246944275901</v>
-      </c>
-      <c r="D49">
-        <v>5.1613803315773499</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>5.7124211298315899</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50">
-        <v>48</v>
+        <v>66.538947797605005</v>
       </c>
       <c r="B50">
-        <v>0.247642529507378</v>
-      </c>
-      <c r="D50">
-        <v>5.7124211298315899</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>2.45121387212422</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51">
-        <v>49</v>
+        <v>0.66796582903151502</v>
       </c>
       <c r="B51">
-        <v>66.538947797605005</v>
-      </c>
-      <c r="D51">
-        <v>2.45121387212422</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>1.79883336480012</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52">
-        <v>50</v>
+        <v>4.9257567603967303</v>
       </c>
       <c r="B52">
-        <v>0.66796582903151502</v>
-      </c>
-      <c r="D52">
-        <v>1.79883336480012</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4">
+        <v>1.87840014773034</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53">
-        <v>51</v>
+        <v>0.81200359801022104</v>
       </c>
       <c r="B53">
-        <v>4.9257567603967303</v>
-      </c>
-      <c r="D53">
-        <v>1.87840014773034</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4">
+        <v>0.85042974269243898</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54">
-        <v>52</v>
+        <v>25.409251824100501</v>
       </c>
       <c r="B54">
-        <v>0.81200359801022104</v>
-      </c>
-      <c r="D54">
-        <v>0.85042974269243898</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4">
+        <v>6.9968526361293</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55">
-        <v>53</v>
+        <v>4.1966915242088803</v>
       </c>
       <c r="B55">
-        <v>25.409251824100501</v>
-      </c>
-      <c r="D55">
-        <v>6.9968526361293</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4">
+        <v>0.12596273026714799</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56">
-        <v>54</v>
+        <v>49.610303162668998</v>
       </c>
       <c r="B56">
-        <v>4.1966915242088803</v>
-      </c>
-      <c r="D56">
-        <v>0.12596273026714799</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4">
+        <v>0.19797875826091499</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57">
-        <v>55</v>
+        <v>3.2808362806664899</v>
       </c>
       <c r="B57">
-        <v>49.610303162668998</v>
-      </c>
-      <c r="D57">
-        <v>0.19797875826091499</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4">
+        <v>0.93301537975266402</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58">
-        <v>56</v>
+        <v>57.1482075551558</v>
       </c>
       <c r="B58">
-        <v>3.2808362806664899</v>
-      </c>
-      <c r="D58">
-        <v>0.93301537975266402</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4">
+        <v>3.4032208348979101</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59">
-        <v>57</v>
+        <v>1.4345334499647799</v>
       </c>
       <c r="B59">
-        <v>57.1482075551558</v>
-      </c>
-      <c r="D59">
-        <v>3.4032208348979101</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4">
+        <v>1.86386722541686</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60">
-        <v>58</v>
+        <v>12.355595155600399</v>
       </c>
       <c r="B60">
-        <v>1.4345334499647799</v>
-      </c>
-      <c r="D60">
-        <v>1.86386722541686</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4">
+        <v>5.7044497966398797</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61">
-        <v>59</v>
+        <v>4.1745234696609099</v>
       </c>
       <c r="B61">
-        <v>12.355595155600399</v>
-      </c>
-      <c r="D61">
-        <v>5.7044497966398797</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4">
+        <v>2.3639576818179502</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62">
-        <v>60</v>
+        <v>40.726378710540303</v>
       </c>
       <c r="B62">
-        <v>4.1745234696609099</v>
-      </c>
-      <c r="D62">
-        <v>2.3639576818179502</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4">
+        <v>5.0301786345108201</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63">
-        <v>61</v>
+        <v>1.4979695280746299</v>
       </c>
       <c r="B63">
-        <v>40.726378710540303</v>
-      </c>
-      <c r="D63">
-        <v>5.0301786345108201</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4">
+        <v>3.22219260478892</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64">
-        <v>62</v>
+        <v>21.770715045222101</v>
       </c>
       <c r="B64">
-        <v>1.4979695280746299</v>
-      </c>
-      <c r="D64">
-        <v>3.22219260478892</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <v>0.121997935003979</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65">
-        <v>63</v>
+        <v>1.37467302637722</v>
       </c>
       <c r="B65">
-        <v>21.770715045222101</v>
-      </c>
-      <c r="D65">
-        <v>0.121997935003979</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <v>8.0858155169137205E-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66">
-        <v>64</v>
+        <v>151.51798851517401</v>
       </c>
       <c r="B66">
-        <v>1.37467302637722</v>
-      </c>
-      <c r="D66">
-        <v>8.0858155169137205E-2</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <v>1.84721653915164</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67">
-        <v>65</v>
+        <v>0.165858090102983</v>
       </c>
       <c r="B67">
-        <v>151.51798851517401</v>
-      </c>
-      <c r="D67">
-        <v>1.84721653915164</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <v>0.57586976651201305</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68">
-        <v>66</v>
+        <v>13.019595189016099</v>
       </c>
       <c r="B68">
-        <v>0.165858090102983</v>
-      </c>
-      <c r="D68">
-        <v>0.57586976651201305</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <v>3.8713930198644402</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69">
-        <v>67</v>
+        <v>0.168540309530995</v>
       </c>
       <c r="B69">
-        <v>13.019595189016099</v>
-      </c>
-      <c r="D69">
-        <v>3.8713930198644402</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <v>4.3896591961474298</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70">
-        <v>68</v>
+        <v>42.089965544559</v>
       </c>
       <c r="B70">
-        <v>0.168540309530995</v>
-      </c>
-      <c r="D70">
-        <v>4.3896591961474298</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <v>2.7623481938002099</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71">
-        <v>69</v>
+        <v>0.65027771372332199</v>
       </c>
       <c r="B71">
-        <v>42.089965544559</v>
-      </c>
-      <c r="D71">
-        <v>2.7623481938002099</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4">
+        <v>1.24382196561398</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72">
-        <v>70</v>
+        <v>32.120849498170799</v>
       </c>
       <c r="B72">
-        <v>0.65027771372332199</v>
-      </c>
-      <c r="D72">
-        <v>1.24382196561398</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4">
+        <v>8.7121751912762804</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73">
-        <v>71</v>
+        <v>0.66695703113857696</v>
       </c>
       <c r="B73">
-        <v>32.120849498170799</v>
-      </c>
-      <c r="D73">
-        <v>8.7121751912762804</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4">
+        <v>1.1751683460342199</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74">
-        <v>72</v>
+        <v>64.504204233337106</v>
       </c>
       <c r="B74">
-        <v>0.66695703113857696</v>
-      </c>
-      <c r="D74">
-        <v>1.1751683460342199</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4">
+        <v>2.8282109344548199E-2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75">
-        <v>73</v>
+        <v>1.5571638866260999</v>
       </c>
       <c r="B75">
-        <v>64.504204233337106</v>
-      </c>
-      <c r="D75">
-        <v>2.8282109344548199E-2</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4">
+        <v>1.70918311615017</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76">
-        <v>74</v>
+        <v>176.99612803049399</v>
       </c>
       <c r="B76">
-        <v>1.5571638866260999</v>
-      </c>
-      <c r="D76">
-        <v>1.70918311615017</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4">
+        <v>3.9222916227767799</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77">
-        <v>75</v>
+        <v>1.5477558320406299</v>
       </c>
       <c r="B77">
-        <v>176.99612803049399</v>
-      </c>
-      <c r="D77">
-        <v>3.9222916227767799</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4">
+        <v>0.398144123806561</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78">
-        <v>76</v>
+        <v>68.355220161484695</v>
       </c>
       <c r="B78">
-        <v>1.5477558320406299</v>
-      </c>
-      <c r="D78">
-        <v>0.398144123806561</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4">
+        <v>1.01268377780992</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79">
-        <v>77</v>
+        <v>0.75734072704903199</v>
       </c>
       <c r="B79">
-        <v>68.355220161484695</v>
-      </c>
-      <c r="D79">
-        <v>1.01268377780992</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4">
+        <v>2.1371536182492501</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80">
-        <v>78</v>
+        <v>27.468868588454601</v>
       </c>
       <c r="B80">
-        <v>0.75734072704903199</v>
-      </c>
-      <c r="D80">
-        <v>2.1371536182492501</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
+        <v>1.6368483427271701</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81">
-        <v>79</v>
+        <v>0.96478955228732699</v>
       </c>
       <c r="B81">
-        <v>27.468868588454601</v>
-      </c>
-      <c r="D81">
-        <v>1.6368483427271701</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
+        <v>1.1325572498401399</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82">
-        <v>80</v>
+        <v>59.188290566155999</v>
       </c>
       <c r="B82">
-        <v>0.96478955228732699</v>
-      </c>
-      <c r="D82">
-        <v>1.1325572498401399</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
+        <v>4.3636904341608798</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83">
-        <v>81</v>
+        <v>3.5587755500081002</v>
       </c>
       <c r="B83">
-        <v>59.188290566155999</v>
-      </c>
-      <c r="D83">
-        <v>4.3636904341608798</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
+        <v>4.0487995903831697</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84">
-        <v>82</v>
+        <v>1.03163258521909</v>
       </c>
       <c r="B84">
-        <v>3.5587755500081002</v>
-      </c>
-      <c r="D84">
-        <v>4.0487995903831697</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4">
+        <v>4.1768312882570298</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85">
-        <v>83</v>
+        <v>1.3997671702560901</v>
       </c>
       <c r="B85">
-        <v>1.03163258521909</v>
-      </c>
-      <c r="D85">
-        <v>4.1768312882570298</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4">
+        <v>1.4411307225840799</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86">
-        <v>84</v>
+        <v>33.8811195447324</v>
       </c>
       <c r="B86">
-        <v>1.3997671702560901</v>
-      </c>
-      <c r="D86">
-        <v>1.4411307225840799</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4">
+        <v>1.4984503017477899</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87">
-        <v>85</v>
+        <v>3.00601367626975E-2</v>
       </c>
       <c r="B87">
-        <v>33.8811195447324</v>
-      </c>
-      <c r="D87">
-        <v>1.4984503017477899</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4">
+        <v>2.5200500962922701</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88">
-        <v>86</v>
+        <v>39.476937304314497</v>
       </c>
       <c r="B88">
-        <v>3.00601367626975E-2</v>
-      </c>
-      <c r="D88">
-        <v>2.5200500962922701</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4">
+        <v>1.5970429524630001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89">
-        <v>87</v>
+        <v>1.48426778810997</v>
       </c>
       <c r="B89">
-        <v>39.476937304314497</v>
-      </c>
-      <c r="D89">
-        <v>1.5970429524630001</v>
-      </c>
-    </row>
-    <row r="90" spans="1:4">
+        <v>2.9606283335321799</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90">
-        <v>88</v>
+        <v>31.530385125909401</v>
       </c>
       <c r="B90">
-        <v>1.48426778810997</v>
-      </c>
-      <c r="D90">
-        <v>2.9606283335321799</v>
-      </c>
-    </row>
-    <row r="91" spans="1:4">
+        <v>1.5056279069883201</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91">
-        <v>89</v>
+        <v>0.71039898268854695</v>
       </c>
       <c r="B91">
-        <v>31.530385125909401</v>
-      </c>
-      <c r="D91">
-        <v>1.5056279069883201</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4">
+        <v>0.46127125902313298</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92">
-        <v>90</v>
+        <v>7.6090039058200798</v>
       </c>
       <c r="B92">
-        <v>0.71039898268854695</v>
-      </c>
-      <c r="D92">
-        <v>0.46127125902313298</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4">
-      <c r="A93">
-        <v>91</v>
-      </c>
-      <c r="B93">
-        <v>7.6090039058200798</v>
-      </c>
-      <c r="D93">
         <v>0.89441001345562299</v>
       </c>
     </row>

</xml_diff>